<commit_message>
dodadeni 2 stud, promena na oceni
</commit_message>
<xml_diff>
--- a/students.csv.xlsx
+++ b/students.csv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilija Ristovski\Desktop\GitHub\ileristovski1-SI_lab1_gr2_173093\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilija Ristovski\SI_lab1_gr2_173093\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F35956-E85E-42FB-827D-5AFE16D0A77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03A8CAC-A2F7-42DC-9F7F-A1491284301E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0CA09F8E-D502-477B-8132-ADB37A004996}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Index</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Ronaldov</t>
+  </si>
+  <si>
+    <t>Petko</t>
+  </si>
+  <si>
+    <t>Stojan</t>
+  </si>
+  <si>
+    <t>Stojanovski</t>
   </si>
 </sst>
 </file>
@@ -436,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A328006-0E1E-4058-AF08-6FE6EECA23CC}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -597,6 +606,58 @@
         <v>7</v>
       </c>
       <c r="H6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>173333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>173001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
     </row>

</xml_diff>